<commit_message>
made anonymous demo version
</commit_message>
<xml_diff>
--- a/Forma.xlsx
+++ b/Forma.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Egle\Documents\excel reader\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Egle\Documents\Python projects\excel reader\Invoice-generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02451836-3B18-4AC0-B7B1-F61E0D5A5DFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A37D5D7D-4F90-43BB-8C98-F1F1804AB5BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,12 +41,6 @@
     <t>SĄSKAITA FAKTŪRA</t>
   </si>
   <si>
-    <t>Tel. Nr.: +370 606 35695</t>
-  </si>
-  <si>
-    <t>El. Paštas:  ilonaieva@gmail.com</t>
-  </si>
-  <si>
     <t>Paslaugos gavėjas:</t>
   </si>
   <si>
@@ -56,34 +50,40 @@
     <t>Paslaugos pavadinimas</t>
   </si>
   <si>
-    <t>Būrelio vadovė: Ilona Sakalauskienė</t>
-  </si>
-  <si>
     <t>1.</t>
   </si>
   <si>
     <t>Kaina Eur</t>
   </si>
   <si>
-    <t>Būrelis ,,Gyvūnėlių mylėtojai",</t>
-  </si>
-  <si>
-    <t>Pastabos: Mokėjimo paskirtyje įrašyti: vaiko vardą, pavardę.</t>
-  </si>
-  <si>
-    <t>Adresas: Miglovaros g. 7- 4, Šiauliai</t>
-  </si>
-  <si>
-    <t>Paslaugos teikėjas: Ilona Sakalauskienė</t>
-  </si>
-  <si>
-    <t>Individualios veiklos vykdymo pažyma Nr. 1389187</t>
-  </si>
-  <si>
-    <t>Banko sąskaita: LT317300010111659884</t>
-  </si>
-  <si>
-    <t>Bankas: Swedbank AB</t>
+    <t>Individualios veiklos vykdymo pažyma Nr. 1234567</t>
+  </si>
+  <si>
+    <t>Adresas: Gatvės g. 1, Miestas</t>
+  </si>
+  <si>
+    <t>Banko sąskaita: LT123456789123456789</t>
+  </si>
+  <si>
+    <t>Bankas: ManoBankas</t>
+  </si>
+  <si>
+    <t>Tel. Nr.: +370 61234567</t>
+  </si>
+  <si>
+    <t>El. Paštas:  paštas@gmail.com</t>
+  </si>
+  <si>
+    <t>Paslauga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pastabos: </t>
+  </si>
+  <si>
+    <t>Paslaugos teikėjas: Vardas Pavardė</t>
+  </si>
+  <si>
+    <t>Vadovė: Vardas Pavardė</t>
   </si>
 </sst>
 </file>
@@ -591,108 +591,108 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
     <col min="2" max="2" width="54" customWidth="1"/>
     <col min="3" max="3" width="21.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" ht="18.5" x14ac:dyDescent="0.9">
       <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B4" s="3"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B5" s="3"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B6" s="3"/>
     </row>
-    <row r="7" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.75">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.75">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.75">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.75">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.75">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.5" thickBot="1" x14ac:dyDescent="0.9"/>
+    <row r="15" spans="1:3" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="A15" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.75">
+      <c r="A16" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="15" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>9</v>
-      </c>
       <c r="C16" s="10"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A17" s="11"/>
       <c r="B17" s="12"/>
       <c r="C17" s="14"/>
     </row>
-    <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:3" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A18" s="8"/>
       <c r="B18" s="1"/>
       <c r="C18" s="2"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A25" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>